<commit_message>
fix make slides e bova11
</commit_message>
<xml_diff>
--- a/avaliacao_estrutura_dados.xlsx
+++ b/avaliacao_estrutura_dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="34">
   <si>
     <t>Gestor</t>
   </si>
@@ -46,79 +46,76 @@
     <t>Etrnty</t>
   </si>
   <si>
-    <t>47.716.356/0001-90</t>
+    <t>47.700.200/0001-10</t>
   </si>
   <si>
     <t>37.525.998/0001-58</t>
   </si>
   <si>
-    <t>38.195.760/0001-74</t>
-  </si>
-  <si>
-    <t>42.831.231/0001-97</t>
-  </si>
-  <si>
-    <t>49.722.651/0001-84</t>
-  </si>
-  <si>
-    <t>24.193.691/0001-55</t>
-  </si>
-  <si>
-    <t>41.409.831/0001-07</t>
-  </si>
-  <si>
-    <t>26.516.247/0001-59</t>
-  </si>
-  <si>
-    <t>35.940.266/0001-07</t>
-  </si>
-  <si>
-    <t>14.146.496/0001-10</t>
-  </si>
-  <si>
-    <t>51.162.466/0001-24</t>
-  </si>
-  <si>
-    <t>41.153.236/0001-45</t>
-  </si>
-  <si>
-    <t>35.617.938/0001-30</t>
+    <t>37.487.439/0001-09</t>
+  </si>
+  <si>
+    <t>51.152.458/0001-05</t>
+  </si>
+  <si>
+    <t>45.089.460/0001-76</t>
+  </si>
+  <si>
+    <t>44.769.980/0001-67</t>
+  </si>
+  <si>
+    <t>34.431.065/0001-03</t>
+  </si>
+  <si>
+    <t>36.318.430/0001-01</t>
+  </si>
+  <si>
+    <t>26.243.348/0001-01</t>
+  </si>
+  <si>
+    <t>25.213.366/0001-70</t>
+  </si>
+  <si>
+    <t>37.367.932/0001-87</t>
+  </si>
+  <si>
+    <t>37.887.412/0001-03</t>
+  </si>
+  <si>
+    <t>BRBOVACTF003</t>
   </si>
   <si>
     <t>SANTANDER CASH BLACK FUNDO DE INVESTIMENTO RENDA FIXA REFERENCIADO DI</t>
   </si>
   <si>
-    <t>IBIUNA HEDGE STC FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>KAPITALO ZETA MERÍDIA FUNDO DE INVESTIMENTO EM COTAS DE FUNDO DE INVESTIMENTOS MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>LEGACY CAPITAL ALPHA FUNDO DE INVESTIMENTO EM COTAS DE FUNDO DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>SPX NIMITZ GRIPEN ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>VINLAND MACRO PLUS ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>XPA HARPIA FIC FIM CP IE</t>
-  </si>
-  <si>
-    <t>GIANT ZARATHUSTRA ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>KADIMA HIGH VOL FUNDO DE INVEST COTAS  FUNDO INVEST MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>IBIUNA LONG SHORT FO FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>RPS TOTAL RETURN ADVISORY D30 FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
-  </si>
-  <si>
-    <t>ABSOLUTE ALPHA MARB ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
+    <t>ENCORE LONG BIAS FC FUNDO DE INVESTIMENTO EM COTAS DE FUNDO DE INVESTIMENTO MULTIMERCADO</t>
+  </si>
+  <si>
+    <t>3 ILHAS FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>AT ADVISORY II FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>DCG ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>DCG ADVISORY I FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>DCG ADVISORY II FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>IBIUNA EQUITIES 30 FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>KIRON FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>NÚCLEO AÇÕES FF FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
+  </si>
+  <si>
+    <t>SHARP EQUITY VALUE ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO EM AÇÕES</t>
   </si>
 </sst>
 </file>
@@ -480,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -532,16 +529,16 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>0.03723484906573235</v>
+        <v>0.005520420788341678</v>
       </c>
       <c r="G2">
-        <v>0.009692520443221886</v>
+        <v>0.009004628880522558</v>
       </c>
       <c r="H2">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I2">
-        <v>0.0003608995357698921</v>
+        <v>4.970934046333859E-05</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -549,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -561,16 +558,16 @@
         <v>24</v>
       </c>
       <c r="F3">
-        <v>0.09875576134972588</v>
+        <v>0.1681477128776219</v>
       </c>
       <c r="G3">
-        <v>-0.008915095191558087</v>
+        <v>0.1270000013724544</v>
       </c>
       <c r="H3">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I3">
-        <v>-0.0008804170131475992</v>
+        <v>0.02135475976623304</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -578,7 +575,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -590,16 +587,16 @@
         <v>25</v>
       </c>
       <c r="F4">
-        <v>0.07543974311210459</v>
+        <v>0.06007207374091752</v>
       </c>
       <c r="G4">
-        <v>-0.01276617124202395</v>
+        <v>0.1419480750279409</v>
       </c>
       <c r="H4">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I4">
-        <v>-0.000963076679023424</v>
+        <v>0.008527115230459761</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -607,7 +604,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -619,16 +616,16 @@
         <v>26</v>
       </c>
       <c r="F5">
-        <v>0.1118488163076545</v>
+        <v>0.1184157220945272</v>
       </c>
       <c r="G5">
-        <v>-0.04895164973774913</v>
+        <v>0.1036407476066392</v>
       </c>
       <c r="H5">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I5">
-        <v>-0.005475184079474144</v>
+        <v>0.01227269396625682</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -636,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -648,16 +645,16 @@
         <v>27</v>
       </c>
       <c r="F6">
-        <v>0.08260326919254654</v>
+        <v>0.1042530342176093</v>
       </c>
       <c r="G6">
-        <v>0.001883440202683939</v>
+        <v>0.1373677863600369</v>
       </c>
       <c r="H6">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I6">
-        <v>0.0001555783180703659</v>
+        <v>0.01432100853179017</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -665,7 +662,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -677,16 +674,16 @@
         <v>28</v>
       </c>
       <c r="F7">
-        <v>0.1087884289190724</v>
+        <v>0.03048630719531616</v>
       </c>
       <c r="G7">
-        <v>-0.002761423069244984</v>
+        <v>0.1351673979025918</v>
       </c>
       <c r="H7">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I7">
-        <v>-0.0003004108772840447</v>
+        <v>0.004120754815249947</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -694,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -706,16 +703,16 @@
         <v>29</v>
       </c>
       <c r="F8">
-        <v>0.04491024920519368</v>
+        <v>0.0164437382267689</v>
       </c>
       <c r="G8">
-        <v>-0.004083201551264515</v>
+        <v>0.1355130842437617</v>
       </c>
       <c r="H8">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I8">
-        <v>-0.0001833775992223228</v>
+        <v>0.002228341683606499</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -723,7 +720,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -735,16 +732,16 @@
         <v>30</v>
       </c>
       <c r="F9">
-        <v>0.1145001798143101</v>
+        <v>0.1566659032739198</v>
       </c>
       <c r="G9">
-        <v>-0.0002683564834884411</v>
+        <v>0.1117154578070505</v>
       </c>
       <c r="H9">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I9">
-        <v>-3.072686561376246E-05</v>
+        <v>0.01750200310700104</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -752,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -764,16 +761,16 @@
         <v>31</v>
       </c>
       <c r="F10">
-        <v>0.03374666689519321</v>
+        <v>0.1455210747581034</v>
       </c>
       <c r="G10">
-        <v>-0.01195879835277891</v>
+        <v>0.1345988338263711</v>
       </c>
       <c r="H10">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I10">
-        <v>-0.0004035695844780151</v>
+        <v>0.01958696695960088</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -781,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -793,16 +790,16 @@
         <v>32</v>
       </c>
       <c r="F11">
-        <v>0.1471825584328852</v>
+        <v>0.1544819140819563</v>
       </c>
       <c r="G11">
-        <v>-0.01545110337347722</v>
+        <v>0.1733180466064985</v>
       </c>
       <c r="H11">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I11">
-        <v>-0.00227413292511936</v>
+        <v>0.0267745035847176</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -810,7 +807,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -822,16 +819,16 @@
         <v>33</v>
       </c>
       <c r="F12">
-        <v>0.07569587175811786</v>
+        <v>0.0400817365426801</v>
       </c>
       <c r="G12">
-        <v>-0.02014676906697044</v>
+        <v>0.1035275090225443</v>
       </c>
       <c r="H12">
-        <v>-0.01179424598082401</v>
+        <v>0.1247611111013232</v>
       </c>
       <c r="I12">
-        <v>-0.00152502724763381</v>
+        <v>0.004149562341561557</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -839,28 +836,28 @@
         <v>9</v>
       </c>
       <c r="B13" s="2">
-        <v>45230</v>
+        <v>45291</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F13">
-        <v>0.08688184335527488</v>
+        <v>0.06257747393100689</v>
       </c>
       <c r="G13">
-        <v>0.003126697077612262</v>
+        <v>0.008931710497727785</v>
       </c>
       <c r="H13">
-        <v>-0.01179424598082401</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I13">
-        <v>0.0002716532057165042</v>
+        <v>0.0005589238808308611</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -868,28 +865,28 @@
         <v>9</v>
       </c>
       <c r="B14" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F14">
-        <v>0.05341857466423781</v>
+        <v>0.1632646241945478</v>
       </c>
       <c r="G14">
-        <v>0.009004628880522558</v>
+        <v>0.03257243561527146</v>
       </c>
       <c r="H14">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I14">
-        <v>0.0004810144401779464</v>
+        <v>0.005317926459828399</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -897,28 +894,28 @@
         <v>9</v>
       </c>
       <c r="B15" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>0.09643005788392822</v>
+        <v>0.05880984136703236</v>
       </c>
       <c r="G15">
-        <v>0.02504719076264617</v>
+        <v>0.04111039283564066</v>
       </c>
       <c r="H15">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I15">
-        <v>0.002415302055071762</v>
+        <v>0.002417695681200411</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -926,28 +923,28 @@
         <v>9</v>
       </c>
       <c r="B16" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F16">
-        <v>0.0764253483919205</v>
+        <v>0.1165832636562356</v>
       </c>
       <c r="G16">
-        <v>0.06348434213946907</v>
+        <v>0.04699893330999827</v>
       </c>
       <c r="H16">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I16">
-        <v>0.004851812965440803</v>
+        <v>0.00547928903364136</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -955,28 +952,28 @@
         <v>9</v>
       </c>
       <c r="B17" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F17">
-        <v>0.1135524631872975</v>
+        <v>0.1014621016604445</v>
       </c>
       <c r="G17">
-        <v>0.06575907846153362</v>
+        <v>0.03498617663035897</v>
       </c>
       <c r="H17">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I17">
-        <v>0.007467105336233904</v>
+        <v>0.003549771009979749</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -984,28 +981,28 @@
         <v>9</v>
       </c>
       <c r="B18" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F18">
-        <v>0.07801167458900016</v>
+        <v>0.02967637710676399</v>
       </c>
       <c r="G18">
-        <v>-0.008583281359309303</v>
+        <v>0.03520285510393517</v>
       </c>
       <c r="H18">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I18">
-        <v>-0.0006695961523082683</v>
+        <v>0.001044693203299152</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1013,28 +1010,28 @@
         <v>9</v>
       </c>
       <c r="B19" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F19">
-        <v>0.1055564932844203</v>
+        <v>0.01599925358097765</v>
       </c>
       <c r="G19">
-        <v>0.01858229364563613</v>
+        <v>0.0347098093226208</v>
       </c>
       <c r="H19">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I19">
-        <v>0.001961481754414715</v>
+        <v>0.0005553310410999922</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1042,28 +1039,28 @@
         <v>9</v>
       </c>
       <c r="B20" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20">
-        <v>0.04178200502672191</v>
+        <v>0.1558111287798582</v>
       </c>
       <c r="G20">
-        <v>-0.02335284996629405</v>
+        <v>0.05765343696306924</v>
       </c>
       <c r="H20">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I20">
-        <v>-0.0009757288946799806</v>
+        <v>0.008983047091254217</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1071,28 +1068,28 @@
         <v>9</v>
       </c>
       <c r="B21" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F21">
-        <v>0.1071316878216128</v>
+        <v>0.1442376025810088</v>
       </c>
       <c r="G21">
-        <v>-0.01778705786627088</v>
+        <v>0.05407617969592371</v>
       </c>
       <c r="H21">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I21">
-        <v>-0.001905557530594294</v>
+        <v>0.007799818516079864</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1100,28 +1097,28 @@
         <v>9</v>
       </c>
       <c r="B22" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F22">
-        <v>0.03259108090217332</v>
+        <v>0.1517001377081059</v>
       </c>
       <c r="G22">
-        <v>0.01382210173719467</v>
+        <v>0.0443058984914102</v>
       </c>
       <c r="H22">
-        <v>0.01409271627016162</v>
+        <v>0.04300970673719795</v>
       </c>
       <c r="I22">
-        <v>0.0004504772359549818</v>
+        <v>0.006721210902428291</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1129,28 +1126,28 @@
         <v>9</v>
       </c>
       <c r="B23" s="2">
-        <v>45260</v>
+        <v>45322</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F23">
-        <v>0.1385074211866267</v>
+        <v>0.05615169929225114</v>
       </c>
       <c r="G23">
-        <v>-0.01210549567772956</v>
+        <v>0.009613807412615527</v>
       </c>
       <c r="H23">
-        <v>0.01409271627016162</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I23">
-        <v>-0.001676700988508178</v>
+        <v>0.0005398316228868021</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1158,28 +1155,28 @@
         <v>9</v>
       </c>
       <c r="B24" s="2">
-        <v>45260</v>
+        <v>45322</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F24">
-        <v>0.07321004509123992</v>
+        <v>0.1364392528324063</v>
       </c>
       <c r="G24">
-        <v>0.01529524819095629</v>
+        <v>0.004462490076883929</v>
       </c>
       <c r="H24">
-        <v>0.01409271627016162</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I24">
-        <v>0.001119765809741616</v>
+        <v>0.0006088588118620708</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1187,28 +1184,28 @@
         <v>9</v>
       </c>
       <c r="B25" s="2">
-        <v>45260</v>
+        <v>45322</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F25">
-        <v>0.08374949838087427</v>
+        <v>0.05538004567252153</v>
       </c>
       <c r="G25">
-        <v>0.0119220550728365</v>
+        <v>-0.04949870886241869</v>
       </c>
       <c r="H25">
-        <v>0.01409271627016162</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I25">
-        <v>0.0009984661320192145</v>
+        <v>-0.002741240757531594</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1216,28 +1213,28 @@
         <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F26">
-        <v>0.09627123469520346</v>
+        <v>0.1138427461683278</v>
       </c>
       <c r="G26">
-        <v>0.008931710497727785</v>
+        <v>-0.01435944752561036</v>
       </c>
       <c r="H26">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I26">
-        <v>0.0008598667975563641</v>
+        <v>-0.001634718939775483</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1245,28 +1242,28 @@
         <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F27">
-        <v>0.08522850436382354</v>
+        <v>0.09693183962435788</v>
       </c>
       <c r="G27">
-        <v>0.04165424775927073</v>
+        <v>-0.03570034658652166</v>
       </c>
       <c r="H27">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I27">
-        <v>0.003550129236922793</v>
+        <v>-0.00346050026985871</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1274,28 +1271,28 @@
         <v>9</v>
       </c>
       <c r="B28" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F28">
-        <v>0.07722282049673856</v>
+        <v>0.0283515679772763</v>
       </c>
       <c r="G28">
-        <v>0.01936075258948167</v>
+        <v>-0.03569235879641464</v>
       </c>
       <c r="H28">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I28">
-        <v>0.001495091921899309</v>
+        <v>-0.001011934336685885</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1303,28 +1300,28 @@
         <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F29">
-        <v>0.1156989440445724</v>
+        <v>0.01528882560824846</v>
       </c>
       <c r="G29">
-        <v>0.02790389559247841</v>
+        <v>-0.03545208255286147</v>
       </c>
       <c r="H29">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I29">
-        <v>0.003228451254779751</v>
+        <v>-0.0005420207075999268</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1332,28 +1329,28 @@
         <v>9</v>
       </c>
       <c r="B30" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F30">
-        <v>0.03591245674243589</v>
+        <v>0.1349162759828932</v>
       </c>
       <c r="G30">
-        <v>0.01640181573114252</v>
+        <v>-0.03355606245351073</v>
       </c>
       <c r="H30">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I30">
-        <v>0.0005890294979420603</v>
+        <v>-0.004527258982877052</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1361,28 +1358,28 @@
         <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F31">
-        <v>0.10657686018842</v>
+        <v>0.1326473152568687</v>
       </c>
       <c r="G31">
-        <v>0.01858586144184149</v>
+        <v>-0.02103852344805579</v>
       </c>
       <c r="H31">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I31">
-        <v>0.001980822756368487</v>
+        <v>-0.00279070365235328</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1390,28 +1387,28 @@
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F32">
-        <v>0.04246193400954094</v>
+        <v>0.13769083808694</v>
       </c>
       <c r="G32">
-        <v>0.02525092469043311</v>
+        <v>-0.0838460094336777</v>
       </c>
       <c r="H32">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I32">
-        <v>0.001072203097885058</v>
+        <v>-0.01154482730916856</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1419,492 +1416,25 @@
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F33">
-        <v>0.1068143381333631</v>
+        <v>0.09235995966667127</v>
       </c>
       <c r="G33">
-        <v>0.005845511774390744</v>
+        <v>-0.0481503529733881</v>
       </c>
       <c r="H33">
-        <v>0.02271243128108269</v>
+        <v>-0.03274741752067933</v>
       </c>
       <c r="I33">
-        <v>0.0006243844712323284</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="2">
-        <v>45291</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34">
-        <v>0.03307088776459066</v>
-      </c>
-      <c r="G34">
-        <v>0.02368600051439707</v>
-      </c>
-      <c r="H34">
-        <v>0.02271243128108269</v>
-      </c>
-      <c r="I34">
-        <v>0.000783317064603662</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="2">
-        <v>45291</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35">
-        <v>0.1434606901822857</v>
-      </c>
-      <c r="G35">
-        <v>0.04491159459671956</v>
-      </c>
-      <c r="H35">
-        <v>0.02271243128108269</v>
-      </c>
-      <c r="I35">
-        <v>0.006443048358032402</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="2">
-        <v>45291</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36">
-        <v>0.07342952997665547</v>
-      </c>
-      <c r="G36">
-        <v>0.01185841988724534</v>
-      </c>
-      <c r="H36">
-        <v>0.02271243128108269</v>
-      </c>
-      <c r="I36">
-        <v>0.0008707581985862492</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="2">
-        <v>45291</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37">
-        <v>0.08393701553481843</v>
-      </c>
-      <c r="G37">
-        <v>0.0110927237053835</v>
-      </c>
-      <c r="H37">
-        <v>0.02271243128108269</v>
-      </c>
-      <c r="I37">
-        <v>0.0009310901219822236</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38">
-        <v>0.1056303112153451</v>
-      </c>
-      <c r="G38">
-        <v>0.009613807412615527</v>
-      </c>
-      <c r="H38">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I38">
-        <v>0.00101550946895897</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39">
-        <v>0.08345664674714633</v>
-      </c>
-      <c r="G39">
-        <v>-0.01390022862260465</v>
-      </c>
-      <c r="H39">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I39">
-        <v>-0.001160066469861289</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40">
-        <v>0.07644953416238227</v>
-      </c>
-      <c r="G40">
-        <v>-0.0030486216274761</v>
-      </c>
-      <c r="H40">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I40">
-        <v>-0.0002330657032579116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41">
-        <v>0.1150469966536185</v>
-      </c>
-      <c r="G41">
-        <v>0.001361028544540677</v>
-      </c>
-      <c r="H41">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I41">
-        <v>0.0001565822464092505</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42">
-        <v>0.03577692925796241</v>
-      </c>
-      <c r="G42">
-        <v>0.003235150404766296</v>
-      </c>
-      <c r="H42">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I42">
-        <v>0.0001157437471701922</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" t="s">
-        <v>28</v>
-      </c>
-      <c r="F43">
-        <v>0.1046662463677446</v>
-      </c>
-      <c r="G43">
-        <v>-0.011017691492333</v>
-      </c>
-      <c r="H43">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I43">
-        <v>-0.00115318041214033</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44">
-        <v>0.04210680606151451</v>
-      </c>
-      <c r="G44">
-        <v>-0.001386753310664401</v>
-      </c>
-      <c r="H44">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I44">
-        <v>-5.839175270730912E-05</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45">
-        <v>0.1050167496587387</v>
-      </c>
-      <c r="G45">
-        <v>-0.009911962346017877</v>
-      </c>
-      <c r="H45">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I45">
-        <v>-0.001040922068318603</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" t="s">
-        <v>31</v>
-      </c>
-      <c r="F46">
-        <v>0.03329680877851054</v>
-      </c>
-      <c r="G46">
-        <v>0.01391501091235048</v>
-      </c>
-      <c r="H46">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I46">
-        <v>0.0004633254574994214</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47">
-        <v>0.1444062524969685</v>
-      </c>
-      <c r="G47">
-        <v>0.01367299485699913</v>
-      </c>
-      <c r="H47">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I47">
-        <v>0.001974465947709568</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>21</v>
-      </c>
-      <c r="E48" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48">
-        <v>0.07141342146513591</v>
-      </c>
-      <c r="G48">
-        <v>-0.02061400915105494</v>
-      </c>
-      <c r="H48">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I48">
-        <v>-0.001472116923590454</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="2">
-        <v>45322</v>
-      </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" t="s">
-        <v>34</v>
-      </c>
-      <c r="F49">
-        <v>0.08277473293098622</v>
-      </c>
-      <c r="G49">
-        <v>-0.006908968908715618</v>
-      </c>
-      <c r="H49">
-        <v>-0.002033890561840224</v>
-      </c>
-      <c r="I49">
-        <v>-0.0005718880562474226</v>
+        <v>-0.00444716465855811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>